<commit_message>
-Version en producción 19-12-2018
</commit_message>
<xml_diff>
--- a/hmm_application/config.xlsx
+++ b/hmm_application/config.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="web_page" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>entity</t>
   </si>
@@ -42,9 +42,6 @@
     <t>CAL_DIST_QUITO_P.CARGA_TOT_1_CAL.AV</t>
   </si>
   <si>
-    <t>INF.GER_DEM-MAX_ELECTRICA DE GUAYAQUIL - EP</t>
-  </si>
-  <si>
     <t>Demanda Empresa Eléctrica Quito</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     </r>
   </si>
   <si>
-    <t>Deamanda Empresa Eléctrica Guayaquil</t>
-  </si>
-  <si>
     <t>despacho</t>
   </si>
   <si>
@@ -135,20 +129,145 @@
     <t>historic</t>
   </si>
   <si>
-    <t>SELECT t.Demanda MW  FROM SIVO.dbo.DV_Demanda t where UNegocio = 'DQUI' and Fecha between '{0}' and '{1}'</t>
-  </si>
-  <si>
-    <t>SELECT t.Demanda MW  FROM SIVO.dbo.DV_Demanda t where UNegocio = 'EGYG' and Fecha between '{0}' and '{1}'</t>
-  </si>
-  <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>SELECT t.Central, t.Unidad, t.MV_Validado,  t.Fecha, t.Hora FROM SIVO.dbo.DV_Generacion t  where t.MV_Validado &gt; 0 and t.Fecha between '{0}' and '{1}'</t>
+  </si>
+  <si>
+    <t>SELECT t.Demanda MW, t.Fecha, t.Hora  FROM SIVO.dbo.DV_Demanda t where UNegocio = 'DQUI' and Fecha between '{0}' and '{1}'</t>
+  </si>
+  <si>
+    <t>SELECT t.Demanda MW, t.Fecha, t.Hora  FROM SIVO.dbo.DV_Demanda t where UNegocio = 'EGYG' and Fecha between '{0}' and '{1}'</t>
+  </si>
+  <si>
+    <t>Demanda CNEL EP Guayaquil</t>
+  </si>
+  <si>
+    <t>centro-sur</t>
+  </si>
+  <si>
+    <t>Demanda EE. Centro Sur</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hmm_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EE.Centro_sur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.pkl</t>
+    </r>
+  </si>
+  <si>
+    <t>CAL_DIST_CENTRSUR_P.CARGA_TOT_1_CAL.AV</t>
+  </si>
+  <si>
+    <t>SELECT t.Demanda MW, t.Fecha, t.Hora  FROM SIVO.dbo.DV_Demanda t where UNegocio = 'DRCS' and Fecha between '{0}' and '{1}'</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Nacional</t>
+  </si>
+  <si>
+    <t>EE. Quito</t>
+  </si>
+  <si>
+    <t>CNEL Guayaquil</t>
+  </si>
+  <si>
+    <t>Centro Sur</t>
+  </si>
+  <si>
+    <t>ambato</t>
+  </si>
+  <si>
+    <t>E.E. Ambato</t>
+  </si>
+  <si>
+    <t>Demanda E.E. Ambato</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hmm_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ambato</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.pkl</t>
+    </r>
+  </si>
+  <si>
+    <t>CAL_DIST_EMELEC_P.CARGA_TOT_1_CAL.AV</t>
+  </si>
+  <si>
+    <t>CAL_DIST_AMBATO_P.CARGA_TOT_1_CAL.AV</t>
+  </si>
+  <si>
+    <t>SELECT t.Demanda MW, t.Fecha, t.Hora  FROM SIVO.dbo.DV_Demanda t where UNegocio = 'DAMB' and Fecha between '{0}' and '{1}'</t>
+  </si>
+  <si>
+    <t>n_comp_min</t>
+  </si>
+  <si>
+    <t>n_comp_max</t>
+  </si>
+  <si>
+    <t>n_interaction</t>
+  </si>
+  <si>
+    <t>Entrenamiento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +291,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFA9B7C6"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -192,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -215,20 +340,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,104 +664,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
-    <col min="6" max="6" width="103.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" customWidth="1"/>
+    <col min="7" max="7" width="128.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>120</v>
+      </c>
+      <c r="J2">
+        <v>160</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>140</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>140</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>140</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F5" s="6"/>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>80</v>
+      </c>
+      <c r="J6">
+        <v>120</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>